<commit_message>
new protocol files for Ryo's screen v2
</commit_message>
<xml_diff>
--- a/ProtocolFiles/EP_Bubble_v003p9.xlsx
+++ b/ProtocolFiles/EP_Bubble_v003p9.xlsx
@@ -404,7 +404,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -573,7 +573,7 @@
         <v>30</v>
       </c>
       <c r="B12" s="8" t="n">
-        <v>3.7</v>
+        <v>3.9</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>5</v>

</xml_diff>